<commit_message>
data path done, and gates done. about to do or gate.
</commit_message>
<xml_diff>
--- a/instrtTable.xlsx
+++ b/instrtTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="1880" yWindow="2300" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="81">
   <si>
     <t>addi</t>
   </si>
@@ -249,6 +249,27 @@
   </si>
   <si>
     <t>101011</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>011001</t>
+  </si>
+  <si>
+    <t>100010</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>101100</t>
   </si>
 </sst>
 </file>
@@ -601,23 +622,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M21" sqref="M21"/>
+      <selection pane="topRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="4"/>
-    <col min="17" max="17" width="10.83203125" style="4"/>
-    <col min="18" max="18" width="10.83203125" style="5"/>
-    <col min="20" max="20" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -676,10 +708,13 @@
         <v>8</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -738,10 +773,13 @@
         <v>38</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -800,10 +838,13 @@
         <v>38</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -814,7 +855,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>38</v>
@@ -823,10 +864,10 @@
         <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>37</v>
@@ -862,10 +903,13 @@
         <v>38</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -876,7 +920,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>38</v>
@@ -885,10 +929,10 @@
         <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>38</v>
@@ -924,10 +968,13 @@
         <v>38</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -986,10 +1033,13 @@
         <v>38</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1050,8 +1100,11 @@
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1110,10 +1163,13 @@
         <v>39</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1172,10 +1228,13 @@
         <v>39</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1236,8 +1295,11 @@
       <c r="T10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1298,8 +1360,11 @@
       <c r="T11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1358,10 +1423,13 @@
         <v>39</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1422,8 +1490,11 @@
       <c r="T13" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1482,10 +1553,13 @@
         <v>38</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1544,10 +1618,13 @@
         <v>38</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1608,8 +1685,11 @@
       <c r="T16" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1668,10 +1748,13 @@
         <v>38</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1730,10 +1813,13 @@
         <v>38</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1792,10 +1878,13 @@
         <v>38</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1854,10 +1943,13 @@
         <v>38</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1867,183 +1959,448 @@
       <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T25" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="T27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U27" s="1" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
single cycle cpu done, start modifing it into 2 stage.
</commit_message>
<xml_diff>
--- a/instrtTable.xlsx
+++ b/instrtTable.xlsx
@@ -122,9 +122,6 @@
     <t>ALUSrc</t>
   </si>
   <si>
-    <t>MemtoReg</t>
-  </si>
-  <si>
     <t>MemWr</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Ext (0 - zero extend, else, sign)</t>
-  </si>
-  <si>
     <t>001000</t>
   </si>
   <si>
@@ -270,6 +264,12 @@
   </si>
   <si>
     <t>101100</t>
+  </si>
+  <si>
+    <t>MemToReg</t>
+  </si>
+  <si>
+    <t>ExtOp (0 - zero extend, else, sign)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,6 +345,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +629,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I31" sqref="I31"/>
+      <selection pane="topRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +649,7 @@
     <col min="18" max="18" width="3.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -663,43 +666,43 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>10</v>
@@ -708,75 +711,75 @@
         <v>8</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -784,64 +787,64 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -849,64 +852,64 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -914,64 +917,64 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -979,64 +982,64 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1044,64 +1047,64 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1109,64 +1112,64 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1174,64 +1177,64 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1239,64 +1242,64 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1304,64 +1307,64 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1369,64 +1372,64 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1434,64 +1437,64 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1499,64 +1502,64 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1564,64 +1567,64 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1629,64 +1632,64 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1694,64 +1697,64 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1759,64 +1762,64 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1824,64 +1827,64 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1889,64 +1892,64 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -1954,64 +1957,64 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2019,64 +2022,64 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2084,64 +2087,64 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2149,64 +2152,64 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2214,64 +2217,64 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2279,64 +2282,64 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -2344,64 +2347,64 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many bug fixed, almost done, final testing stage
</commit_message>
<xml_diff>
--- a/instrtTable.xlsx
+++ b/instrtTable.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="82">
   <si>
     <t>addi</t>
   </si>
@@ -212,9 +212,6 @@
     <t>nPCsel (0 - pc+4; 1 - branch; 2 - j/jal; 3 - jr)</t>
   </si>
   <si>
-    <t>111111</t>
-  </si>
-  <si>
     <t>100011</t>
   </si>
   <si>
@@ -270,6 +267,12 @@
   </si>
   <si>
     <t>ExtOp (0 - zero extend, else, sign)</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>001111</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +350,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G29" sqref="G29"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +648,7 @@
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="14" max="14" width="38" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -652,7 +658,7 @@
     <col min="21" max="21" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -687,7 +693,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -711,13 +717,16 @@
         <v>8</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -781,8 +790,11 @@
       <c r="U2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -846,8 +858,11 @@
       <c r="U3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -858,7 +873,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>37</v>
@@ -911,8 +926,11 @@
       <c r="U4" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -923,7 +941,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
@@ -976,8 +994,11 @@
       <c r="U5" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1041,8 +1062,11 @@
       <c r="U6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1106,8 +1130,11 @@
       <c r="U7" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1171,8 +1198,11 @@
       <c r="U8" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1236,8 +1266,11 @@
       <c r="U9" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1301,8 +1334,11 @@
       <c r="U10" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1366,8 +1402,11 @@
       <c r="U11" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1431,13 +1470,16 @@
       <c r="U12" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
@@ -1497,12 +1539,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
@@ -1561,8 +1603,11 @@
       <c r="U14" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1570,11 +1615,11 @@
         <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="E15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1627,18 +1672,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>36</v>
@@ -1692,7 +1737,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1700,11 +1745,11 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1757,18 +1802,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>36</v>
@@ -1822,18 +1867,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>36</v>
@@ -1887,7 +1932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1895,10 +1940,10 @@
         <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>36</v>
@@ -1952,7 +1997,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -2017,7 +2062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2025,7 +2070,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>57</v>
@@ -2082,7 +2127,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2147,12 +2192,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
@@ -2211,13 +2256,16 @@
       <c r="U24" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>40</v>
@@ -2276,8 +2324,11 @@
       <c r="U25" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="V25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2285,11 +2336,11 @@
         <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E26" s="1" t="s">
         <v>37</v>
       </c>
@@ -2342,7 +2393,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2350,10 +2401,10 @@
         <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>36</v>
@@ -2405,6 +2456,80 @@
       </c>
       <c r="U27" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D29" s="7">
+        <f>COUNTIF(D2:D27,"="&amp;"1")</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" ref="E29:U29" si="0">COUNTIF(E2:E27,"="&amp;"1")</f>
+        <v>9</v>
+      </c>
+      <c r="F29" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L29" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M29" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N29" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O29" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P29" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q29" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R29" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T29" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="U29" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all test added and tested, everything works. the test is after the submission, but the submission works perfectly, this commit added tests and not to be summitted. just committing for record keeping.
</commit_message>
<xml_diff>
--- a/instrtTable.xlsx
+++ b/instrtTable.xlsx
@@ -635,7 +635,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,6 +656,7 @@
     <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -1538,6 +1539,9 @@
       <c r="U13" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1671,6 +1675,9 @@
       <c r="U15" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1736,6 +1743,9 @@
       <c r="U16" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1801,6 +1811,9 @@
       <c r="U17" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1866,6 +1879,9 @@
       <c r="U18" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1931,6 +1947,9 @@
       <c r="U19" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1996,6 +2015,9 @@
       <c r="U20" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -2061,6 +2083,9 @@
       <c r="U21" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -2126,6 +2151,9 @@
       <c r="U22" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -2191,6 +2219,9 @@
       <c r="U23" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -2392,6 +2423,9 @@
       <c r="U26" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -2456,6 +2490,9 @@
       </c>
       <c r="U27" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>